<commit_message>
RPPL-2104: Remove fields from device manifests which echo default values (#349)
</commit_message>
<xml_diff>
--- a/docs/device_manifest_default_values.xlsx
+++ b/docs/device_manifest_default_values.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAD6D749-2DAC-4DDE-BCCB-1224A2044DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pahear000/dev/code/eos-ripple/docs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFED7795-6377-374F-AF58-3B7B88E12D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-102220" yWindow="-7120" windowWidth="50920" windowHeight="27940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="168">
   <si>
     <t>Device Manifest Default Values</t>
   </si>
@@ -378,9 +383,6 @@
     <t>endpoint</t>
   </si>
   <si>
-    <t>"https://collector-dev.sift.comcast.com/events/entos"</t>
-  </si>
-  <si>
     <t>api_key</t>
   </si>
   <si>
@@ -535,6 +537,9 @@
   </si>
   <si>
     <t>* Atomic Default refers to fields within a struct which have a default value only if the entire struct is absent from the manifest.</t>
+  </si>
+  <si>
+    <t>https://collector-dev.sift.comcast.com/events/entos</t>
   </si>
 </sst>
 </file>
@@ -544,7 +549,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -564,16 +569,19 @@
       <sz val="12"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Courier New"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -586,12 +594,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="16"/>
@@ -628,39 +637,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1004,1442 +1002,1397 @@
   <dimension ref="A1:D117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="97.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="97.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="15" customFormat="1" ht="21">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:4" s="9" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="9" customFormat="1" ht="13.5">
-      <c r="C2" s="10"/>
-    </row>
-    <row r="3" spans="1:4" s="4" customFormat="1">
-      <c r="A3" s="4" t="s">
+    <row r="2" spans="1:4" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="3" customFormat="1">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="7" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="7" t="s">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="11" t="b">
+      <c r="C15" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="7" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="7" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="7" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="7" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="7" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="7" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="7" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="11" t="b">
+      <c r="C29" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="8" t="s">
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="17">
+      <c r="C30" s="10">
         <v>5</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="7" t="s">
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="11" t="b">
+      <c r="C31" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="7" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="11" t="b">
+      <c r="C32" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="7" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="11" t="b">
+      <c r="C33" s="6" t="b">
         <v>1</v>
       </c>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="7" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="11" t="b">
+      <c r="C34" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="7" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="11" t="b">
+      <c r="C35" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="7" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="11" t="b">
+      <c r="C36" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="7" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="11" t="b">
+      <c r="C37" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="7" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="11" t="b">
+      <c r="C38" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="7" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="11" t="b">
+      <c r="C39" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="7" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="11" t="b">
+      <c r="C40" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="7" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="11" t="b">
+      <c r="C41" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="7" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="11" t="b">
+      <c r="C42" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="7" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="11" t="b">
+      <c r="C43" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="7" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="7" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="7" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="7" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="7" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="11"/>
+      <c r="C48" s="6"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="7" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="7" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="6" t="s">
         <v>64</v>
       </c>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="7" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="6" t="s">
         <v>66</v>
       </c>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="7" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="6" t="s">
         <v>68</v>
       </c>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="7" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="6" t="s">
         <v>70</v>
       </c>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="7" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="6" t="s">
         <v>64</v>
       </c>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="7" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="6" t="s">
         <v>72</v>
       </c>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="7" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C56" s="18" t="s">
+      <c r="C56" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="7" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C57" s="18" t="s">
+      <c r="C57" s="6" t="s">
         <v>76</v>
       </c>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="7" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C58" s="18" t="s">
+      <c r="C58" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="7" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C59" s="18" t="s">
+      <c r="C59" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="7" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C60" s="18" t="s">
+      <c r="C60" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="7" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="18" t="s">
+      <c r="C61" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="13" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C62" s="19" t="s">
+      <c r="C62" s="11" t="s">
         <v>86</v>
       </c>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="13" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C63" s="19" t="s">
+      <c r="C63" s="11" t="s">
         <v>88</v>
       </c>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="13" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="11" t="s">
         <v>91</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="13" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="C65" s="11" t="s">
         <v>93</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="13" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B66" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C66" s="19" t="s">
+      <c r="C66" s="11" t="s">
         <v>96</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="13" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B67" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C67" s="19" t="s">
+      <c r="C67" s="11" t="s">
         <v>96</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="13" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C68" s="19" t="b">
+      <c r="C68" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="13" t="s">
+      <c r="D68" s="1"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C69" s="19" t="s">
+      <c r="C69" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="13" t="s">
+      <c r="D69" s="1"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B70" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C70" s="19">
+      <c r="C70" s="11">
         <v>14400</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="13" t="s">
+      <c r="D70" s="1"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B71" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C71" s="19">
+      <c r="C71" s="11">
         <v>30</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="13" t="s">
+      <c r="D71" s="1"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C72" s="19">
+      <c r="C72" s="11">
         <v>600</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="13" t="s">
+      <c r="D72" s="1"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="B73" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="C73" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="13" t="s">
+      <c r="D73" s="1"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="B74" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C74" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="13" t="s">
+      <c r="D74" s="1"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="B75" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C75" s="11">
+      <c r="C75" s="6">
         <v>1000</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="13" t="s">
+      <c r="D75" s="1"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B76" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C76" s="11">
+      <c r="C76" s="6">
         <v>32000</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="13" t="s">
+      <c r="D76" s="1"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="B77" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C77" s="11">
+      <c r="C77" s="6">
         <v>300</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="13" t="s">
+      <c r="D77" s="1"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B78" s="7" t="s">
+      <c r="B78" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C78" s="19" t="s">
+      <c r="C78" s="11" t="s">
         <v>112</v>
       </c>
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="7" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="B79" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C79" s="18" t="s">
+      <c r="C79" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="D79" s="1"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B80" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="7" t="s">
+      <c r="C80" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D80" s="1"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B80" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C80" s="18" t="s">
+      <c r="B81" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D80" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="7" t="s">
+      <c r="C81" s="6">
+        <v>3</v>
+      </c>
+      <c r="D81" s="1"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="B82" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C81" s="18">
-        <v>3</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="7" t="s">
+      <c r="C82" s="6">
+        <v>20</v>
+      </c>
+      <c r="D82" s="1"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="B83" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C82" s="18">
-        <v>20</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="7" t="s">
+      <c r="C83" s="6">
+        <v>30</v>
+      </c>
+      <c r="D83" s="1"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="B84" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C83" s="18">
-        <v>30</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B84" s="7" t="s">
+      <c r="C84" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D84" s="1"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C84" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D84" s="1"/>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="7" t="s">
+      <c r="B85" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B85" s="7" t="s">
+      <c r="C85" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="C85" s="18" t="s">
-        <v>124</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B86" s="7" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C86" s="6" t="s">
         <v>125</v>
-      </c>
-      <c r="C86" s="18" t="s">
-        <v>126</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B87" s="7" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C87" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C87" s="18" t="s">
+      <c r="D87" s="1"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D87" s="1"/>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="7" t="s">
+      <c r="C88" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D88" s="1"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D89" s="1"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D90" s="1"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C91" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D91" s="1"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C92" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D92" s="1"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D93" s="1"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B88" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C88" s="11" t="s">
+      <c r="B94" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C94" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D88" s="1"/>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C89" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D89" s="1"/>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C90" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="D90" s="1"/>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C91" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D91" s="1"/>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C92" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D92" s="1"/>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C93" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D93" s="1"/>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="7" t="s">
+      <c r="D94" s="1"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B94" s="7" t="s">
+      <c r="B95" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D95" s="1"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C94" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D94" s="1"/>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="7" t="s">
+      <c r="B96" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D96" s="1"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B95" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C95" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D95" s="1"/>
-    </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="B96" s="7" t="s">
+      <c r="B97" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C96" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D96" s="1"/>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="7" t="s">
+      <c r="C97" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D97" s="1"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B97" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C97" s="11" t="s">
+      <c r="B98" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D97" s="1"/>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B98" s="7" t="s">
+      <c r="C98" s="6">
+        <v>10</v>
+      </c>
+      <c r="D98" s="1"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C98" s="11">
-        <v>10</v>
-      </c>
-      <c r="D98" s="1"/>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="7" t="s">
+      <c r="B99" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B99" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C99" s="11" t="s">
+      <c r="C99" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="C100" s="11" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C100" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B101" s="7" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D101" s="1"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B102" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C101" s="11" t="s">
+      <c r="C102" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D101" s="1"/>
-    </row>
-    <row r="102" spans="1:4">
-      <c r="A102" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B102" s="7" t="s">
+      <c r="D102" s="1"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C102" s="11" t="s">
+      <c r="B103" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C103" s="6">
+        <v>0</v>
+      </c>
+      <c r="D103" s="1"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C104" s="6">
+        <v>0</v>
+      </c>
+      <c r="D104" s="1"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C105" s="6">
+        <v>0</v>
+      </c>
+      <c r="D105" s="1"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C106" s="6">
+        <v>0</v>
+      </c>
+      <c r="D106" s="1"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C107" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D102" s="1"/>
-    </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B103" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C103" s="11">
+      <c r="D107" s="1"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C108" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="D103" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B104" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C104" s="11">
-        <v>0</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
-      <c r="A105" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B105" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C105" s="11">
-        <v>0</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B106" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C106" s="11">
-        <v>0</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4">
-      <c r="A107" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B107" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="C107" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="A108" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B108" s="7" t="s">
+      <c r="D108" s="1"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C108" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D108" s="1"/>
-    </row>
-    <row r="109" spans="1:4">
-      <c r="A109" s="7" t="s">
+      <c r="B109" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B109" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C109" s="11" t="s">
+      <c r="C109" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
-      <c r="A110" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B110" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="C110" s="11" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C110" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
-      <c r="A111" s="7" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B111" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B111" s="7" t="s">
+      <c r="C111" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D111" s="1"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B112" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C111" s="11" t="s">
+      <c r="C112" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D111" s="1"/>
-    </row>
-    <row r="112" spans="1:4">
-      <c r="A112" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="B112" s="7" t="s">
+      <c r="D112" s="1"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B113" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C112" s="11" t="s">
+      <c r="C113" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D113" s="1"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C114" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D112" s="1"/>
-    </row>
-    <row r="113" spans="1:4">
-      <c r="A113" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="B113" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C113" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D113" s="1"/>
-    </row>
-    <row r="114" spans="1:4">
-      <c r="A114" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="B114" s="7" t="s">
+      <c r="D114" s="1"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>165</v>
       </c>
-      <c r="C114" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D114" s="1"/>
-    </row>
-    <row r="116" spans="1:4">
-      <c r="A116" t="s">
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
-      <c r="A117" t="s">
-        <v>167</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C79" r:id="rId1" xr:uid="{FF0A0F14-5F0A-3844-B0E9-2149882482BB}"/>
+  </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape"/>

</xml_diff>